<commit_message>
Add Zip code and phone number Validation
</commit_message>
<xml_diff>
--- a/employee_data_2.xlsx
+++ b/employee_data_2.xlsx
@@ -1,41 +1,117 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepanshu\Desktop\Repo\Employee Database\Employee-Database\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B77B1A-0ABD-4CF8-ACCD-C4AA85689AAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11400" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>Employee ID</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Shaun</t>
+  </si>
+  <si>
+    <t>Pollock</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>541-754-3010</t>
+  </si>
+  <si>
+    <t>Beverly</t>
+  </si>
+  <si>
+    <t>Merritt</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>652-328-4125</t>
+  </si>
+  <si>
+    <t>Christopher</t>
+  </si>
+  <si>
+    <t>Cramer</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>124-858-4525</t>
+  </si>
+  <si>
+    <t>Dale</t>
+  </si>
+  <si>
+    <t>Addison</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>646-165-5825</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -54,14 +130,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -349,170 +434,122 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F8" sqref="A6:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="14.85546875" customWidth="1" style="2" min="1" max="1"/>
-    <col width="17.5703125" customWidth="1" style="2" min="2" max="2"/>
-    <col width="14.140625" customWidth="1" style="2" min="3" max="3"/>
-    <col width="13.28515625" customWidth="1" style="2" min="4" max="4"/>
-    <col width="10.7109375" customWidth="1" style="2" min="5" max="5"/>
-    <col width="16.5703125" customWidth="1" style="2" min="6" max="6"/>
+    <col min="1" max="1" width="14.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Employee ID</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>First Name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Last Name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>State</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Zip Code</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Phone Number</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="n"/>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1"/>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>100150</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Shaun</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Pollock</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Florida</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
         <v>50210</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>541-754-3010</t>
-        </is>
+      <c r="F2" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>100151</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Beverly</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Merritt</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>California</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
         <v>80542</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>652-328-4125</t>
-        </is>
+      <c r="F3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>100152</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Christopher</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Cramer</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>IL</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
         <v>60007</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>124-858-4525</t>
-        </is>
+      <c r="F4" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>100153</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Dale</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Addison</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>UT</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
         <v>84606</v>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>646-165-5825</t>
-        </is>
+      <c r="F5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged Module 1 into Module 2, Removed the long message in Module4 with a try/except and cleaned up the code a little.
</commit_message>
<xml_diff>
--- a/employee_data_2.xlsx
+++ b/employee_data_2.xlsx
@@ -1,117 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepanshu\Desktop\Repo\Employee Database\Employee-Database\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B77B1A-0ABD-4CF8-ACCD-C4AA85689AAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11400" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>Employee ID</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Zip Code</t>
-  </si>
-  <si>
-    <t>Phone Number</t>
-  </si>
-  <si>
-    <t>Shaun</t>
-  </si>
-  <si>
-    <t>Pollock</t>
-  </si>
-  <si>
-    <t>Florida</t>
-  </si>
-  <si>
-    <t>541-754-3010</t>
-  </si>
-  <si>
-    <t>Beverly</t>
-  </si>
-  <si>
-    <t>Merritt</t>
-  </si>
-  <si>
-    <t>California</t>
-  </si>
-  <si>
-    <t>652-328-4125</t>
-  </si>
-  <si>
-    <t>Christopher</t>
-  </si>
-  <si>
-    <t>Cramer</t>
-  </si>
-  <si>
-    <t>IL</t>
-  </si>
-  <si>
-    <t>124-858-4525</t>
-  </si>
-  <si>
-    <t>Dale</t>
-  </si>
-  <si>
-    <t>Addison</t>
-  </si>
-  <si>
-    <t>UT</t>
-  </si>
-  <si>
-    <t>646-165-5825</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -130,23 +54,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -434,122 +349,226 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F8" sqref="A6:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="2" customWidth="1"/>
+    <col width="14.85546875" customWidth="1" style="2" min="1" max="1"/>
+    <col width="17.5703125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="14.140625" customWidth="1" style="2" min="3" max="3"/>
+    <col width="13.28515625" customWidth="1" style="2" min="4" max="4"/>
+    <col width="10.7109375" customWidth="1" style="2" min="5" max="5"/>
+    <col width="16.5703125" customWidth="1" style="2" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Employee ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>State</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Zip Code</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Phone Number</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>100150</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Shaun</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Pollock</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Florida</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>50210</v>
       </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>541-754-3010</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>100151</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Beverly</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Merritt</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>California</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
         <v>80542</v>
       </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>652-328-4125</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>100152</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Christopher</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Cramer</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>IL</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>60007</v>
       </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>124-858-4525</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
         <v>100153</v>
       </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Dale</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Addison</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>UT</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
         <v>84606</v>
       </c>
-      <c r="F5" t="s">
-        <v>21</v>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>646-165-5825</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>100154</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>George</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Washinton</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Arizona</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>73828</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>787-585-5545</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>100155</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Barry</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Oliver</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Arizona</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>54796</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>265-859-4215</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>